<commit_message>
games and courses updated
</commit_message>
<xml_diff>
--- a/assets/courses/courses.xlsx
+++ b/assets/courses/courses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\TheCabbarGithub\thecabbar.github.io\courses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\TheCabbarGithub\thecabbar.github.io\assets\courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE31C5F-B8F1-4CFF-84A0-4E6B6FC4A4FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B446D5-B841-48EF-919E-5A9003FDF81D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -686,11 +686,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -735,6 +750,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,7 +1041,7 @@
   <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,10 +1051,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -1773,7 +1794,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A83:B83"/>
@@ -1781,15 +1810,6 @@
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A50:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>